<commit_message>
display data from db for customer + employee page
</commit_message>
<xml_diff>
--- a/src/assets/DB/DB_table.xlsx
+++ b/src/assets/DB/DB_table.xlsx
@@ -757,7 +757,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -834,7 +834,7 @@
         <v>100</v>
       </c>
       <c r="G2" s="3">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="H2" s="3">
         <v>320</v>
@@ -869,7 +869,7 @@
         <v>200</v>
       </c>
       <c r="G3" s="3">
-        <v>620000</v>
+        <v>62000</v>
       </c>
       <c r="H3" s="3">
         <v>330</v>
@@ -904,7 +904,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="3">
-        <v>320000</v>
+        <v>32000</v>
       </c>
       <c r="H4" s="3">
         <v>340</v>
@@ -939,7 +939,7 @@
         <v>100</v>
       </c>
       <c r="G5" s="3">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="H5" s="3">
         <v>320</v>
@@ -974,7 +974,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="3">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="H6" s="3">
         <v>320</v>
@@ -1009,7 +1009,7 @@
         <v>100</v>
       </c>
       <c r="G7" s="3">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="H7" s="3">
         <v>320</v>
@@ -1044,7 +1044,7 @@
         <v>100</v>
       </c>
       <c r="G8" s="3">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="H8" s="3">
         <v>320</v>
@@ -1079,7 +1079,7 @@
         <v>100</v>
       </c>
       <c r="G9" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H9" s="3">
         <v>220</v>
@@ -1114,7 +1114,7 @@
         <v>97</v>
       </c>
       <c r="G10" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H10" s="3">
         <v>220</v>
@@ -1149,7 +1149,7 @@
         <v>100</v>
       </c>
       <c r="G11" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H11" s="3">
         <v>220</v>
@@ -1184,7 +1184,7 @@
         <v>100</v>
       </c>
       <c r="G12" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H12" s="3">
         <v>220</v>
@@ -1219,7 +1219,7 @@
         <v>100</v>
       </c>
       <c r="G13" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H13" s="3">
         <v>220</v>
@@ -1254,7 +1254,7 @@
         <v>100</v>
       </c>
       <c r="G14" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H14" s="3">
         <v>220</v>
@@ -1289,7 +1289,7 @@
         <v>95</v>
       </c>
       <c r="G15" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H15" s="3">
         <v>220</v>
@@ -1324,7 +1324,7 @@
         <v>100</v>
       </c>
       <c r="G16" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H16" s="3">
         <v>220</v>
@@ -1359,7 +1359,7 @@
         <v>100</v>
       </c>
       <c r="G17" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H17" s="3">
         <v>220</v>
@@ -1394,7 +1394,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="3">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="H18" s="3">
         <v>220</v>
@@ -1418,7 +1418,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
update backend for employee - addList
</commit_message>
<xml_diff>
--- a/src/assets/DB/DB_table.xlsx
+++ b/src/assets/DB/DB_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12260" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12260" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -591,7 +591,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -756,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1418,7 +1418,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1676,23 +1676,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1718,6 +1721,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1726,7 +1730,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1800,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1828,18 +1832,18 @@
         <v>25</v>
       </c>
       <c r="C2" s="3">
-        <v>123456</v>
+        <v>123457</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
-        <v>789012</v>
+        <v>123457</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="3">
-        <v>789012</v>
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>